<commit_message>
Updated calibration curve with real data.
</commit_message>
<xml_diff>
--- a/synbiochemdev/calibration/calibration.xlsx
+++ b/synbiochemdev/calibration/calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28308"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="0" windowWidth="17040" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="calibration.txt" sheetId="1" r:id="rId1"/>
@@ -150,25 +150,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.25</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.0</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -180,25 +180,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.33683188888434</c:v>
+                  <c:v>0.0632</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.769582572062488</c:v>
+                  <c:v>0.0725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.331765291524256</c:v>
+                  <c:v>0.1126</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.966210620522951</c:v>
+                  <c:v>0.1344</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.2658920937912</c:v>
+                  <c:v>0.6075</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30.3028823359453</c:v>
+                  <c:v>0.583</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.8895441</c:v>
+                  <c:v>1.0714</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -213,11 +213,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2120590776"/>
-        <c:axId val="-2146497032"/>
+        <c:axId val="2137193448"/>
+        <c:axId val="2038500616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2120590776"/>
+        <c:axId val="2137193448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -227,12 +227,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146497032"/>
+        <c:crossAx val="2038500616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2146497032"/>
+        <c:axId val="2038500616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -243,7 +243,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2120590776"/>
+        <c:crossAx val="2137193448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -622,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -640,58 +640,114 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>0.33683188888434001</v>
+        <v>6.3200000000000006E-2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>0.76958257206248781</v>
+        <v>7.2499999999999995E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>1.3317652915242559</v>
+        <v>0.11260000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>6.9662106205229515</v>
+        <v>0.13439999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="B6">
-        <v>10.265892093791198</v>
+        <v>0.60750000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="B7">
-        <v>30.302882335945299</v>
+        <v>0.58299999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="B8">
-        <v>56.889544100000002</v>
+        <v>1.0713999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>1.1227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>500</v>
+      </c>
+      <c r="B10">
+        <v>5.1289999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>500</v>
+      </c>
+      <c r="B11">
+        <v>5.4231999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>10.389200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>1000</v>
+      </c>
+      <c r="B13">
+        <v>10.5105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>5000</v>
+      </c>
+      <c r="B14">
+        <v>46.726199999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>5000</v>
+      </c>
+      <c r="B15">
+        <v>51.118200000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>